<commit_message>
Updating test cases for store and user
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Pet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="User" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="69">
   <si>
     <t xml:space="preserve">Sl.No</t>
   </si>
@@ -140,6 +141,93 @@
   </si>
   <si>
     <t xml:space="preserve">own</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userNameAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstNameAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastNameAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passwordAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phoneAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userStatusAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loginPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user,loginPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id,userName,firstName,lastName,email,password,phone,userStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bell1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test12</t>
   </si>
 </sst>
 </file>
@@ -149,7 +237,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -171,8 +259,15 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,7 +277,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FF5EB91E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5EB91E"/>
+        <bgColor rgb="FF81D41A"/>
       </patternFill>
     </fill>
   </fills>
@@ -220,7 +321,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,6 +331,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,7 +406,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF5EB91E"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -312,11 +425,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.39"/>
@@ -834,4 +947,303 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.94"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" display="tom@gmail.com"/>
+    <hyperlink ref="K4" r:id="rId2" display="tom@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>